<commit_message>
commited changes for sigin xlsx
</commit_message>
<xml_diff>
--- a/UploadData/Sigin.xlsx
+++ b/UploadData/Sigin.xlsx
@@ -38,9 +38,6 @@
     <t>Server=PC43\SQLEXPRESS;Database=NH1QCCybAdmin280422;uid=sa;pwd=;Max Pool Size=1000;Connection TimeOut= 3000;</t>
   </si>
   <si>
-    <t>super</t>
-  </si>
-  <si>
     <t>Name@642</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>CTPL Unit2</t>
+  </si>
+  <si>
+    <t>supers</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,10 +396,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -407,16 +407,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sigin file data correction
</commit_message>
<xml_diff>
--- a/UploadData/Sigin.xlsx
+++ b/UploadData/Sigin.xlsx
@@ -53,7 +53,7 @@
     <t>CTPL Unit2</t>
   </si>
   <si>
-    <t>supers</t>
+    <t>super</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>